<commit_message>
function for automatic excel calculations
</commit_message>
<xml_diff>
--- a/9. excel/transactions.xlsx
+++ b/9. excel/transactions.xlsx
@@ -13,14 +13,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">Transaction_id</t>
   </si>
@@ -30,6 +30,9 @@
   <si>
     <t xml:space="preserve">Price</t>
   </si>
+  <si>
+    <t xml:space="preserve">Correct Price</t>
+  </si>
 </sst>
 </file>
 
@@ -38,7 +41,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -59,6 +62,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -103,8 +112,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -117,7 +130,345 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF878787"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FFC0504D"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF9BBB59"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF4F81BD"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4f81bd"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4f81bd"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="c0504d"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="9bbb59"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.355</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.255</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.164</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="150"/>
+        <c:overlap val="0"/>
+        <c:axId val="29556828"/>
+        <c:axId val="17615388"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="29556828"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="878787"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="17615388"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="17615388"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="878787"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="878787"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="29556828"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>523080</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>98640</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="3251160" y="162360"/>
+        <a:ext cx="5399640" cy="2699640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -125,59 +476,71 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
         <v>1001</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>5.95</v>
       </c>
+      <c r="D2" s="1" t="n">
+        <v>5.355</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
         <v>1002</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>6.95</v>
       </c>
+      <c r="D3" s="1" t="n">
+        <v>6.255</v>
+      </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
         <v>1003</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>7.96</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>7.164</v>
       </c>
     </row>
   </sheetData>
@@ -185,8 +548,9 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>